<commit_message>
added files to AssociateGpsToRoute use case
</commit_message>
<xml_diff>
--- a/UseCase/AssociateGpsToRoute/address_book_sample.xlsx
+++ b/UseCase/AssociateGpsToRoute/address_book_sample.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drago\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Oleg_Route4me\Json Schemas\curl examples\UseCase\AssociateGpsToRoute\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21168" windowHeight="10140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Address Book Sample" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -966,8 +966,36 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1278,11 +1306,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="4" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1314,7 +1354,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1346,7 +1386,7 @@
         <v>5435</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1378,7 +1418,7 @@
         <v>5367</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1410,7 +1450,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1442,7 +1482,7 @@
         <v>4578</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1474,7 +1514,7 @@
         <v>4235</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1506,7 +1546,7 @@
         <v>2631</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -1538,7 +1578,7 @@
         <v>9087</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -1570,7 +1610,7 @@
         <v>4684</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -1602,7 +1642,7 @@
         <v>3636</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -1634,7 +1674,7 @@
         <v>2135</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -1666,7 +1706,7 @@
         <v>2564</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -1698,7 +1738,7 @@
         <v>3535</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -1730,7 +1770,7 @@
         <v>2234</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>91</v>
       </c>
@@ -1762,7 +1802,7 @@
         <v>2131</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>97</v>
       </c>
@@ -1794,7 +1834,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>103</v>
       </c>
@@ -1826,7 +1866,7 @@
         <v>9864</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>109</v>
       </c>
@@ -1858,7 +1898,7 @@
         <v>4225</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>115</v>
       </c>
@@ -1890,7 +1930,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>121</v>
       </c>
@@ -1922,7 +1962,7 @@
         <v>4321</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>127</v>
       </c>
@@ -1954,7 +1994,7 @@
         <v>5621</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>133</v>
       </c>

</xml_diff>